<commit_message>
Auto-committed on 2023/02/20 週一 17:13:51.94
</commit_message>
<xml_diff>
--- a/Program/Other/LY006_底稿_B117關係人明細表.xlsx
+++ b/Program/Other/LY006_底稿_B117關係人明細表.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845CA8E6-AD56-4DDC-BD11-31D026DCE314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7580"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B117關係人明細表" sheetId="3" r:id="rId1"/>
@@ -220,12 +221,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>張舜雯</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0" shapeId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1065,7 +1066,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1367,11 +1368,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1380,7 +1381,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1389,10 +1390,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1401,161 +1402,71 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1564,28 +1475,112 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="18" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="5"/>
-    <cellStyle name="一般 3" xfId="3"/>
-    <cellStyle name="一般_半年報檢查報表-壽險" xfId="4"/>
-    <cellStyle name="一般_非RBC相關亦未修訂報表-壽險" xfId="2"/>
+    <cellStyle name="一般 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="一般 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="一般_半年報檢查報表-壽險" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="一般_非RBC相關亦未修訂報表-壽險" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="千分位" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="16">
@@ -6184,88 +6179,88 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table122" displayName="Table122" ref="A2:B17" totalsRowShown="0">
-  <autoFilter ref="A2:B17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table122" displayName="Table122" ref="A2:B17" totalsRowShown="0">
+  <autoFilter ref="A2:B17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="代號"/>
-    <tableColumn id="2" name="說明"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="代號"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="說明"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table125" displayName="Table125" ref="D2:E20" totalsRowShown="0">
-  <autoFilter ref="D2:E20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table125" displayName="Table125" ref="D2:E20" totalsRowShown="0">
+  <autoFilter ref="D2:E20" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="代號" dataDxfId="15"/>
-    <tableColumn id="2" name="說明"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="代號" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="說明"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table121" displayName="Table121" ref="J2:K6" totalsRowShown="0">
-  <autoFilter ref="J2:K6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table121" displayName="Table121" ref="J2:K6" totalsRowShown="0">
+  <autoFilter ref="J2:K6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="代號" dataDxfId="14"/>
-    <tableColumn id="2" name="說明"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="代號" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="說明"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table120" displayName="Table120" ref="G2:H9" totalsRowShown="0">
-  <autoFilter ref="G2:H9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table120" displayName="Table120" ref="G2:H9" totalsRowShown="0">
+  <autoFilter ref="G2:H9" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="代號" dataDxfId="13"/>
-    <tableColumn id="2" name="說明"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="代號" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="說明"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table134" displayName="Table134" ref="J13:K16" totalsRowShown="0">
-  <autoFilter ref="J13:K16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table134" displayName="Table134" ref="J13:K16" totalsRowShown="0">
+  <autoFilter ref="J13:K16" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="代號" dataDxfId="12"/>
-    <tableColumn id="2" name="說明"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="代號" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="說明"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table126" displayName="Table126" ref="M5:N13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="M5:N13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table126" displayName="Table126" ref="M5:N13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="M5:N13" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="代號" dataDxfId="9"/>
-    <tableColumn id="2" name="說明" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="代號" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="說明" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table127" displayName="Table127" ref="M17:N20" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="M17:N20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table127" displayName="Table127" ref="M17:N20" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="M17:N20" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="代號" dataDxfId="5"/>
-    <tableColumn id="2" name="說明" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="代號" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="說明" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table128" displayName="Table128" ref="M23:N31" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="M23:N31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table128" displayName="Table128" ref="M23:N31" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="M23:N31" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="代號" dataDxfId="1"/>
-    <tableColumn id="2" name="說明" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="代號" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="說明" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6567,368 +6562,1536 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="37" style="13" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" style="41" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="15.6328125" style="63" customWidth="1"/>
-    <col min="10" max="10" width="47.08984375" style="13" customWidth="1"/>
-    <col min="11" max="11" width="17.08984375" style="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.453125" style="13" customWidth="1"/>
-    <col min="13" max="13" width="50.36328125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="13"/>
+    <col min="1" max="1" width="9.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="37" style="11" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="29" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="35" customWidth="1"/>
+    <col min="10" max="10" width="47.109375" style="11" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="50.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="39" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A2" s="13" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="62"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="44" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A4" s="13" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="44" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B5" s="15"/>
-    </row>
-    <row r="6" spans="1:13" s="61" customFormat="1" ht="27" x14ac:dyDescent="0.4">
-      <c r="A6" s="16" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+    </row>
+    <row r="6" spans="1:13" s="34" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="46" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="53" customFormat="1" ht="15.5" x14ac:dyDescent="0.4">
-      <c r="A7" s="54" t="s">
+    <row r="7" spans="1:13" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="55" t="s">
+      <c r="I7" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="59" t="s">
+      <c r="K7" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="54" t="s">
+      <c r="L7" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="54" t="s">
+      <c r="M7" s="49" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="50"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="52"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
       <c r="G8" s="52"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" s="68" t="s">
+      <c r="H8" s="53"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10"/>
-      <c r="D10" s="40"/>
-      <c r="E10"/>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="67" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A12" s="67" t="s">
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A13" s="67" t="s">
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A14" s="67" t="s">
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A15" s="71" t="s">
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A16" s="71" t="s">
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" s="66" t="s">
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" s="66" t="s">
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="66" t="s">
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="66" t="s">
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A21" s="66" t="s">
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="66"/>
-      <c r="L21" s="66"/>
-      <c r="M21" s="66"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A22" s="66" t="s">
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="61"/>
+      <c r="M21" s="61"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="69"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="66"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A23" s="66" t="s">
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-    </row>
-    <row r="24" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="66" t="s">
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+    </row>
+    <row r="24" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="66"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A25" s="67" t="s">
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="63"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="39"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A27" s="44" t="s">
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="39"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="47" t="s">
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="G27" s="47"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="47" t="s">
+      <c r="G27" s="67"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="L27" s="48"/>
-      <c r="M27" s="49"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="70"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="39"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="39"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="42"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="39"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="41"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="39"/>
+      <c r="M40" s="39"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="42"/>
+      <c r="L41" s="39"/>
+      <c r="M41" s="39"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="39"/>
+      <c r="M42" s="39"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="39"/>
+      <c r="M43" s="39"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="42"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="42"/>
+      <c r="L45" s="39"/>
+      <c r="M45" s="39"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="42"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="39"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="39"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="42"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="39"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="39"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="41"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="42"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="39"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" s="39"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="42"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="39"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="39"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="42"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="39"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="39"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="39"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="39"/>
+      <c r="K51" s="42"/>
+      <c r="L51" s="39"/>
+      <c r="M51" s="39"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="39"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="39"/>
+      <c r="M52" s="39"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="39"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="39"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="39"/>
+      <c r="M53" s="39"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="39"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="42"/>
+      <c r="L54" s="39"/>
+      <c r="M54" s="39"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" s="39"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="41"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="42"/>
+      <c r="L55" s="39"/>
+      <c r="M55" s="39"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="39"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="42"/>
+      <c r="L56" s="39"/>
+      <c r="M56" s="39"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" s="39"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="41"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="42"/>
+      <c r="L57" s="39"/>
+      <c r="M57" s="39"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" s="39"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="39"/>
+      <c r="M58" s="39"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" s="39"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
+      <c r="I59" s="41"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="39"/>
+      <c r="M59" s="39"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" s="39"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="41"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="42"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="39"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" s="39"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="41"/>
+      <c r="J61" s="39"/>
+      <c r="K61" s="42"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="39"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" s="39"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="41"/>
+      <c r="J62" s="39"/>
+      <c r="K62" s="42"/>
+      <c r="L62" s="39"/>
+      <c r="M62" s="39"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A63" s="39"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="41"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="42"/>
+      <c r="L63" s="39"/>
+      <c r="M63" s="39"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A64" s="39"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
+      <c r="I64" s="41"/>
+      <c r="J64" s="39"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="39"/>
+      <c r="M64" s="39"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A65" s="39"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="39"/>
+      <c r="I65" s="41"/>
+      <c r="J65" s="39"/>
+      <c r="K65" s="42"/>
+      <c r="L65" s="39"/>
+      <c r="M65" s="39"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A66" s="39"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="39"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="39"/>
+      <c r="K66" s="42"/>
+      <c r="L66" s="39"/>
+      <c r="M66" s="39"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A67" s="39"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="41"/>
+      <c r="J67" s="39"/>
+      <c r="K67" s="42"/>
+      <c r="L67" s="39"/>
+      <c r="M67" s="39"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A68" s="39"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="40"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="39"/>
+      <c r="I68" s="41"/>
+      <c r="J68" s="39"/>
+      <c r="K68" s="42"/>
+      <c r="L68" s="39"/>
+      <c r="M68" s="39"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A69" s="39"/>
+      <c r="B69" s="39"/>
+      <c r="C69" s="39"/>
+      <c r="D69" s="40"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="39"/>
+      <c r="H69" s="39"/>
+      <c r="I69" s="41"/>
+      <c r="J69" s="39"/>
+      <c r="K69" s="42"/>
+      <c r="L69" s="39"/>
+      <c r="M69" s="39"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A70" s="39"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="40"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="41"/>
+      <c r="J70" s="39"/>
+      <c r="K70" s="42"/>
+      <c r="L70" s="39"/>
+      <c r="M70" s="39"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A71" s="39"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="41"/>
+      <c r="J71" s="39"/>
+      <c r="K71" s="42"/>
+      <c r="L71" s="39"/>
+      <c r="M71" s="39"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A72" s="39"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="39"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="39"/>
+      <c r="I72" s="41"/>
+      <c r="J72" s="39"/>
+      <c r="K72" s="42"/>
+      <c r="L72" s="39"/>
+      <c r="M72" s="39"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A73" s="39"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="40"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="39"/>
+      <c r="H73" s="39"/>
+      <c r="I73" s="41"/>
+      <c r="J73" s="39"/>
+      <c r="K73" s="42"/>
+      <c r="L73" s="39"/>
+      <c r="M73" s="39"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A74" s="39"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="40"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="39"/>
+      <c r="H74" s="39"/>
+      <c r="I74" s="41"/>
+      <c r="J74" s="39"/>
+      <c r="K74" s="42"/>
+      <c r="L74" s="39"/>
+      <c r="M74" s="39"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A75" s="39"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="39"/>
+      <c r="I75" s="41"/>
+      <c r="J75" s="39"/>
+      <c r="K75" s="42"/>
+      <c r="L75" s="39"/>
+      <c r="M75" s="39"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A76" s="39"/>
+      <c r="B76" s="39"/>
+      <c r="C76" s="39"/>
+      <c r="D76" s="40"/>
+      <c r="E76" s="39"/>
+      <c r="F76" s="39"/>
+      <c r="G76" s="39"/>
+      <c r="H76" s="39"/>
+      <c r="I76" s="41"/>
+      <c r="J76" s="39"/>
+      <c r="K76" s="42"/>
+      <c r="L76" s="39"/>
+      <c r="M76" s="39"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A77" s="39"/>
+      <c r="B77" s="39"/>
+      <c r="C77" s="39"/>
+      <c r="D77" s="40"/>
+      <c r="E77" s="39"/>
+      <c r="F77" s="39"/>
+      <c r="G77" s="39"/>
+      <c r="H77" s="39"/>
+      <c r="I77" s="41"/>
+      <c r="J77" s="39"/>
+      <c r="K77" s="42"/>
+      <c r="L77" s="39"/>
+      <c r="M77" s="39"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A78" s="39"/>
+      <c r="B78" s="39"/>
+      <c r="C78" s="39"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="39"/>
+      <c r="F78" s="39"/>
+      <c r="G78" s="39"/>
+      <c r="H78" s="39"/>
+      <c r="I78" s="41"/>
+      <c r="J78" s="39"/>
+      <c r="K78" s="42"/>
+      <c r="L78" s="39"/>
+      <c r="M78" s="39"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A79" s="39"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39"/>
+      <c r="G79" s="39"/>
+      <c r="H79" s="39"/>
+      <c r="I79" s="41"/>
+      <c r="J79" s="39"/>
+      <c r="K79" s="42"/>
+      <c r="L79" s="39"/>
+      <c r="M79" s="39"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A80" s="39"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="39"/>
+      <c r="D80" s="40"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="39"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="39"/>
+      <c r="I80" s="41"/>
+      <c r="J80" s="39"/>
+      <c r="K80" s="42"/>
+      <c r="L80" s="39"/>
+      <c r="M80" s="39"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A81" s="39"/>
+      <c r="B81" s="39"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="40"/>
+      <c r="E81" s="39"/>
+      <c r="F81" s="39"/>
+      <c r="G81" s="39"/>
+      <c r="H81" s="39"/>
+      <c r="I81" s="41"/>
+      <c r="J81" s="39"/>
+      <c r="K81" s="42"/>
+      <c r="L81" s="39"/>
+      <c r="M81" s="39"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A82" s="39"/>
+      <c r="B82" s="39"/>
+      <c r="C82" s="39"/>
+      <c r="D82" s="40"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="39"/>
+      <c r="G82" s="39"/>
+      <c r="H82" s="39"/>
+      <c r="I82" s="41"/>
+      <c r="J82" s="39"/>
+      <c r="K82" s="42"/>
+      <c r="L82" s="39"/>
+      <c r="M82" s="39"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A83" s="39"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="40"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
+      <c r="G83" s="39"/>
+      <c r="H83" s="39"/>
+      <c r="I83" s="41"/>
+      <c r="J83" s="39"/>
+      <c r="K83" s="42"/>
+      <c r="L83" s="39"/>
+      <c r="M83" s="39"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A84" s="39"/>
+      <c r="B84" s="39"/>
+      <c r="C84" s="39"/>
+      <c r="D84" s="40"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+      <c r="G84" s="39"/>
+      <c r="H84" s="39"/>
+      <c r="I84" s="41"/>
+      <c r="J84" s="39"/>
+      <c r="K84" s="42"/>
+      <c r="L84" s="39"/>
+      <c r="M84" s="39"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A85" s="39"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="40"/>
+      <c r="E85" s="39"/>
+      <c r="F85" s="39"/>
+      <c r="G85" s="39"/>
+      <c r="H85" s="39"/>
+      <c r="I85" s="41"/>
+      <c r="J85" s="39"/>
+      <c r="K85" s="42"/>
+      <c r="L85" s="39"/>
+      <c r="M85" s="39"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A86" s="39"/>
+      <c r="B86" s="39"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="39"/>
+      <c r="H86" s="39"/>
+      <c r="I86" s="41"/>
+      <c r="J86" s="39"/>
+      <c r="K86" s="42"/>
+      <c r="L86" s="39"/>
+      <c r="M86" s="39"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A87" s="39"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="39"/>
+      <c r="H87" s="39"/>
+      <c r="I87" s="41"/>
+      <c r="J87" s="39"/>
+      <c r="K87" s="42"/>
+      <c r="L87" s="39"/>
+      <c r="M87" s="39"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A88" s="39"/>
+      <c r="B88" s="39"/>
+      <c r="C88" s="39"/>
+      <c r="D88" s="40"/>
+      <c r="E88" s="39"/>
+      <c r="F88" s="39"/>
+      <c r="G88" s="39"/>
+      <c r="H88" s="39"/>
+      <c r="I88" s="41"/>
+      <c r="J88" s="39"/>
+      <c r="K88" s="42"/>
+      <c r="L88" s="39"/>
+      <c r="M88" s="39"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A89" s="39"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="40"/>
+      <c r="E89" s="39"/>
+      <c r="F89" s="39"/>
+      <c r="G89" s="39"/>
+      <c r="H89" s="39"/>
+      <c r="I89" s="41"/>
+      <c r="J89" s="39"/>
+      <c r="K89" s="42"/>
+      <c r="L89" s="39"/>
+      <c r="M89" s="39"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A90" s="39"/>
+      <c r="B90" s="39"/>
+      <c r="C90" s="39"/>
+      <c r="D90" s="40"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="39"/>
+      <c r="G90" s="39"/>
+      <c r="H90" s="39"/>
+      <c r="I90" s="41"/>
+      <c r="J90" s="39"/>
+      <c r="K90" s="42"/>
+      <c r="L90" s="39"/>
+      <c r="M90" s="39"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A91" s="39"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="40"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="39"/>
+      <c r="H91" s="39"/>
+      <c r="I91" s="41"/>
+      <c r="J91" s="39"/>
+      <c r="K91" s="42"/>
+      <c r="L91" s="39"/>
+      <c r="M91" s="39"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A92" s="39"/>
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="40"/>
+      <c r="E92" s="39"/>
+      <c r="F92" s="39"/>
+      <c r="G92" s="39"/>
+      <c r="H92" s="39"/>
+      <c r="I92" s="41"/>
+      <c r="J92" s="39"/>
+      <c r="K92" s="42"/>
+      <c r="L92" s="39"/>
+      <c r="M92" s="39"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A93" s="39"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="39"/>
+      <c r="D93" s="40"/>
+      <c r="E93" s="39"/>
+      <c r="F93" s="39"/>
+      <c r="G93" s="39"/>
+      <c r="H93" s="39"/>
+      <c r="I93" s="41"/>
+      <c r="J93" s="39"/>
+      <c r="K93" s="42"/>
+      <c r="L93" s="39"/>
+      <c r="M93" s="39"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:M8"/>
+  <autoFilter ref="A6:M8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="16">
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A25:F25"/>
@@ -6959,7 +8122,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="工作表8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6969,17 +8132,17 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" customWidth="1"/>
-    <col min="2" max="2" width="18.6328125" customWidth="1"/>
-    <col min="3" max="3" width="7.6328125" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" customWidth="1"/>
-    <col min="5" max="6" width="21.6328125" customWidth="1"/>
-    <col min="7" max="7" width="45.08984375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7002,8 +8165,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="A2" s="19">
+    <row r="2" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -7021,12 +8184,12 @@
       <c r="F2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="85" x14ac:dyDescent="0.4">
-      <c r="A3" s="19">
+    <row r="3" spans="1:7" ht="81" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -7048,8 +8211,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="A4" s="19">
+    <row r="4" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -7067,8 +8230,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.4">
-      <c r="A5" s="19">
+    <row r="5" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -7086,8 +8249,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.4">
-      <c r="A6" s="19">
+    <row r="6" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -7103,8 +8266,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="19">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -7118,8 +8281,8 @@
       <c r="F7" s="5"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="A8" s="19">
+    <row r="8" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -7135,8 +8298,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="19">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -7152,8 +8315,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="19">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -7169,8 +8332,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="19">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -7186,8 +8349,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="A12" s="19">
+    <row r="12" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -7205,8 +8368,8 @@
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="68" x14ac:dyDescent="0.4">
-      <c r="A13" s="19">
+    <row r="13" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -7222,8 +8385,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="A14" s="19">
+    <row r="14" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -7239,202 +8402,198 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="15"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="26" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="26" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B21" s="72" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-    </row>
-    <row r="22" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="72" t="s">
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+    </row>
+    <row r="22" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-    </row>
-    <row r="23" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="72" t="s">
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+    </row>
+    <row r="23" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-    </row>
-    <row r="24" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="72" t="s">
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+    </row>
+    <row r="24" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-    </row>
-    <row r="25" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="66" t="s">
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+    </row>
+    <row r="25" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-    </row>
-    <row r="26" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="66" t="s">
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+    </row>
+    <row r="26" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-    </row>
-    <row r="27" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="67" t="s">
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+    </row>
+    <row r="27" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B28" s="67" t="s">
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B29" s="67" t="s">
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-    </row>
-    <row r="30" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="67" t="s">
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+    </row>
+    <row r="30" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-    </row>
-    <row r="31" spans="1:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="67" t="s">
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+    </row>
+    <row r="31" spans="1:7" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-    </row>
-    <row r="32" spans="1:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="67" t="s">
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+    </row>
+    <row r="32" spans="1:7" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B33" s="67" t="s">
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A34" s="14"/>
-      <c r="B34" s="72" t="s">
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A35" s="14"/>
-      <c r="B35" s="72" t="s">
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B36" s="13"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -7465,7 +8624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7475,621 +8634,621 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.26953125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="3.08984375" style="29" customWidth="1"/>
-    <col min="4" max="4" width="3.453125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" style="29" customWidth="1"/>
-    <col min="6" max="6" width="2" style="29" customWidth="1"/>
-    <col min="7" max="7" width="3.08984375" style="29" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="2.36328125" style="29" customWidth="1"/>
-    <col min="10" max="10" width="4" style="29" customWidth="1"/>
-    <col min="11" max="11" width="24.26953125" style="29" customWidth="1"/>
-    <col min="12" max="12" width="6.6328125" style="29" customWidth="1"/>
-    <col min="13" max="13" width="6.36328125" style="36" customWidth="1"/>
-    <col min="14" max="14" width="72.6328125" style="29" customWidth="1"/>
-    <col min="15" max="15" width="7" style="29" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="29"/>
+    <col min="1" max="1" width="4.21875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="2" style="19" customWidth="1"/>
+    <col min="7" max="7" width="3.109375" style="19" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" style="19" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="4" style="19" customWidth="1"/>
+    <col min="11" max="11" width="24.21875" style="19" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" style="25" customWidth="1"/>
+    <col min="14" max="14" width="72.6640625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7" style="19" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="M1" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="M2" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="O2" s="21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="43" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="M3" s="29"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A4" s="30" t="s">
+      <c r="M3" s="19"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="43" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="M4" s="42" t="s">
+      <c r="M4" s="30" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="43" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="43" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="N6" s="35" t="s">
+      <c r="N6" s="24" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="43" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="M7" s="39" t="s">
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="M7" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="N7" s="35" t="s">
+      <c r="N7" s="24" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="34" x14ac:dyDescent="0.4">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:15" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="43" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="M8" s="39" t="s">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="M8" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="N8" s="35" t="s">
+      <c r="N8" s="24" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="51" x14ac:dyDescent="0.4">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:15" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="43" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="M9" s="39" t="s">
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="M9" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="N9" s="35" t="s">
+      <c r="N9" s="24" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="43" t="s">
+      <c r="C10" s="20"/>
+      <c r="D10" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="M10" s="39" t="s">
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="M10" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="N10" s="35" t="s">
+      <c r="N10" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="43" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="M11" s="39" t="s">
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="M11" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="N11" s="35" t="s">
+      <c r="N11" s="24" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="43" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="J12" s="30" t="s">
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="J12" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="K12" s="30"/>
-      <c r="M12" s="39" t="s">
+      <c r="K12" s="20"/>
+      <c r="M12" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="N12" s="35" t="s">
+      <c r="N12" s="24" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A13" s="30" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="43" t="s">
+      <c r="C13" s="22"/>
+      <c r="D13" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="J13" s="30" t="s">
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="J13" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="30" t="s">
+      <c r="K13" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="M13" s="39" t="s">
+      <c r="M13" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="N13" s="35" t="s">
+      <c r="N13" s="24" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="43" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="J14" s="43" t="s">
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="J14" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="K14" s="32" t="s">
+      <c r="K14" s="22" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="43" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="J15" s="43" t="s">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="J15" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="K15" s="30" t="s">
+      <c r="K15" s="20" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A16" s="30" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="43" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="J16" s="43" t="s">
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="J16" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="K16" s="30" t="s">
+      <c r="K16" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="M16" s="42" t="s">
+      <c r="M16" s="30" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A17" s="30" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="43" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="M17" s="38" t="s">
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="M17" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="N17" s="35" t="s">
+      <c r="N17" s="24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="C18" s="34"/>
-      <c r="D18" s="43" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C18"/>
+      <c r="D18" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="M18" s="38" t="s">
+      <c r="M18" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="N18" s="35" t="s">
+      <c r="N18" s="24" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="C19" s="34"/>
-      <c r="D19" s="43" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C19"/>
+      <c r="D19" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="M19" s="38" t="s">
+      <c r="M19" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="N19" s="35" t="s">
+      <c r="N19" s="24" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="34" x14ac:dyDescent="0.4">
-      <c r="C20" s="34"/>
-      <c r="D20" s="43" t="s">
+    <row r="20" spans="1:14" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="C20"/>
+      <c r="D20" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="M20" s="38" t="s">
+      <c r="M20" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="N20" s="35" t="s">
+      <c r="N20" s="24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="C21" s="34"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="C22" s="34"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="M22" s="42" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C21"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C22"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="M22" s="30" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="C23" s="34"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="M23" s="38" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C23"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="M23" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="N23" s="35" t="s">
+      <c r="N23" s="24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="M24" s="38" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M24" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="N24" s="35" t="s">
+      <c r="N24" s="24" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="M25" s="38" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M25" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="N25" s="35" t="s">
+      <c r="N25" s="24" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="M26" s="38" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M26" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="N26" s="35" t="s">
+      <c r="N26" s="24" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="M27" s="38" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M27" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="N27" s="35" t="s">
+      <c r="N27" s="24" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="M28" s="38" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M28" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="N28" s="35" t="s">
+      <c r="N28" s="24" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="M29" s="38" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M29" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="N29" s="35" t="s">
+      <c r="N29" s="24" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="M30" s="38" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M30" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="N30" s="35" t="s">
+      <c r="N30" s="24" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="M31" s="38" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M31" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="N31" s="35" t="s">
+      <c r="N31" s="24" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>